<commit_message>
Better handle duplicate data validation ranges
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -1055,33 +1055,33 @@
       <x:formula1>1.1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="notEqual" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
+      <x:formula1>2.2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
+      <x:formula1>3.3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+      <x:formula1>4.4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
+      <x:formula1>5.5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
+      <x:formula1>6.6</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
+      <x:formula1>7.7</x:formula1>
+      <x:formula2>8.8</x:formula2>
+    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="notBetween" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="H1:H12">
       <x:formula1>9.9</x:formula1>
       <x:formula2>10.1</x:formula2>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
-      <x:formula1>3.3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
-      <x:formula1>7.7</x:formula1>
-      <x:formula2>8.8</x:formula2>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
-      <x:formula1>4.4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="notEqual" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
-      <x:formula1>2.2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
-      <x:formula1>6.6</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
-      <x:formula1>5.5</x:formula1>
-      <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>